<commit_message>
add new export files
</commit_message>
<xml_diff>
--- a/allPages/allPagesEN-SEO.xlsx
+++ b/allPages/allPagesEN-SEO.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="208">
   <si>
     <t>Date</t>
   </si>
@@ -100,6 +100,27 @@
     <t>air cargo transportation Ukraine, air delivery to Ukraine, international air delivery, transportation of cargo by air, air logistics Ukraine, express air delivery, air freight, air cargo transportation, air logistics, air cargo transportation, air transportation from China, air transportation to Europe, air cargo delivery, air freight, air transportation of dangerous goods</t>
   </si>
   <si>
+    <t>11.07.2024</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1.com</t>
+  </si>
+  <si>
+    <t>1.com/7</t>
+  </si>
+  <si>
+    <t>777</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
     <t>https://t-h-logistics.com/en/truck</t>
   </si>
   <si>
@@ -587,6 +608,33 @@
   </si>
   <si>
     <t>Odesa, ports, export, agricultural products, grain, Ukraine, food security</t>
+  </si>
+  <si>
+    <t>17/05/2023</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>superblogs.com.ua</t>
+  </si>
+  <si>
+    <t>https:/superblogs.com.ua/post4.html</t>
+  </si>
+  <si>
+    <t>таможенне оформления 5</t>
+  </si>
+  <si>
+    <t>17/05/2022</t>
+  </si>
+  <si>
+    <t>Doska Obyavleniy</t>
+  </si>
+  <si>
+    <t>https:/superblogs.com.ua/post5.html</t>
+  </si>
+  <si>
+    <t>таможенне оформления 6</t>
   </si>
 </sst>
 </file>
@@ -963,7 +1011,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:K64"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="11" width="20" customWidth="1"/>
@@ -1187,25 +1235,25 @@
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="H7" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="I7" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="J7" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="K7" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1213,13 +1261,13 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -1245,16 +1293,16 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
@@ -1280,16 +1328,16 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
@@ -1315,16 +1363,16 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -1350,16 +1398,16 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -1385,16 +1433,16 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -1420,16 +1468,16 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -1455,16 +1503,16 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
@@ -1490,16 +1538,16 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -1525,16 +1573,16 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
@@ -1560,16 +1608,16 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
@@ -1595,16 +1643,16 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D19" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E19" t="s">
         <v>12</v>
@@ -1630,16 +1678,16 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="E20" t="s">
         <v>12</v>
@@ -1665,16 +1713,16 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="D21" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E21" t="s">
         <v>12</v>
@@ -1700,16 +1748,16 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E22" t="s">
         <v>12</v>
@@ -1735,16 +1783,16 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="D23" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="E23" t="s">
         <v>12</v>
@@ -1770,16 +1818,16 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D24" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="E24" t="s">
         <v>12</v>
@@ -1805,16 +1853,16 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C25" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D25" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="E25" t="s">
         <v>12</v>
@@ -1840,16 +1888,16 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="D26" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="E26" t="s">
         <v>12</v>
@@ -1875,16 +1923,16 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C27" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="D27" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="E27" t="s">
         <v>12</v>
@@ -1910,16 +1958,16 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B28" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="C28" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="D28" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="E28" t="s">
         <v>12</v>
@@ -1945,16 +1993,16 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B29" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C29" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D29" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -1980,16 +2028,16 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="C30" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="D30" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="E30" t="s">
         <v>12</v>
@@ -2015,16 +2063,16 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B31" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="C31" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D31" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E31" t="s">
         <v>12</v>
@@ -2050,16 +2098,16 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B32" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="C32" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="D32" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -2085,16 +2133,16 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B33" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="C33" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D33" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="E33" t="s">
         <v>12</v>
@@ -2120,16 +2168,16 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B34" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="C34" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="D34" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -2155,16 +2203,16 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B35" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="C35" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="D35" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
@@ -2225,7 +2273,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B37" t="s">
         <v>12</v>
@@ -2260,16 +2308,16 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B38" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C38" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D38" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="E38" t="s">
         <v>12</v>
@@ -2295,16 +2343,16 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="C39" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="D39" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -2330,16 +2378,16 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C40" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="D40" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="E40" t="s">
         <v>12</v>
@@ -2365,16 +2413,16 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B41" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C41" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="D41" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="E41" t="s">
         <v>12</v>
@@ -2400,16 +2448,16 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B42" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="C42" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="D42" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="E42" t="s">
         <v>12</v>
@@ -2470,7 +2518,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="B44" t="s">
         <v>12</v>
@@ -2505,16 +2553,16 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B45" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C45" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="D45" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="E45" t="s">
         <v>12</v>
@@ -2575,7 +2623,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="B47" t="s">
         <v>12</v>
@@ -2613,13 +2661,13 @@
         <v>13</v>
       </c>
       <c r="B48" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C48" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="D48" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E48" t="s">
         <v>12</v>
@@ -2645,16 +2693,16 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B49" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C49" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="D49" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="E49" t="s">
         <v>12</v>
@@ -2680,16 +2728,16 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="B50" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="C50" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="D50" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="E50" t="s">
         <v>12</v>
@@ -2715,16 +2763,16 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B51" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C51" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="D51" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="E51" t="s">
         <v>12</v>
@@ -2750,16 +2798,16 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="B52" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="C52" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D52" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="E52" t="s">
         <v>12</v>
@@ -2820,7 +2868,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B54" t="s">
         <v>12</v>
@@ -2855,16 +2903,16 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B55" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="C55" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="D55" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="E55" t="s">
         <v>12</v>
@@ -2890,16 +2938,16 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B56" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="C56" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="D56" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="E56" t="s">
         <v>12</v>
@@ -2925,16 +2973,16 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B57" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="C57" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="D57" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="E57" t="s">
         <v>12</v>
@@ -2960,16 +3008,16 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B58" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="C58" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="D58" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="E58" t="s">
         <v>12</v>
@@ -2995,16 +3043,16 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B59" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="C59" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="D59" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="E59" t="s">
         <v>12</v>
@@ -3030,16 +3078,16 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B60" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="C60" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="D60" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="E60" t="s">
         <v>12</v>
@@ -3065,16 +3113,16 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B61" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="C61" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="D61" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="E61" t="s">
         <v>12</v>
@@ -3100,37 +3148,37 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B62" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="C62" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="D62" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="E62" t="s">
-        <v>12</v>
+        <v>199</v>
       </c>
       <c r="F62" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="G62" t="s">
-        <v>12</v>
+        <v>200</v>
       </c>
       <c r="H62" t="s">
-        <v>12</v>
+        <v>201</v>
       </c>
       <c r="I62" t="s">
-        <v>12</v>
+        <v>202</v>
       </c>
       <c r="J62" t="s">
-        <v>12</v>
-      </c>
-      <c r="K62" t="s">
-        <v>12</v>
+        <v>203</v>
+      </c>
+      <c r="K62">
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -3147,24 +3195,59 @@
         <v>12</v>
       </c>
       <c r="E63" t="s">
-        <v>12</v>
+        <v>204</v>
       </c>
       <c r="F63" t="s">
-        <v>12</v>
+        <v>205</v>
       </c>
       <c r="G63" t="s">
-        <v>12</v>
+        <v>200</v>
       </c>
       <c r="H63" t="s">
-        <v>12</v>
+        <v>201</v>
       </c>
       <c r="I63" t="s">
-        <v>12</v>
+        <v>206</v>
       </c>
       <c r="J63" t="s">
-        <v>12</v>
-      </c>
-      <c r="K63" t="s">
+        <v>207</v>
+      </c>
+      <c r="K63">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" t="s">
+        <v>12</v>
+      </c>
+      <c r="E64" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" t="s">
+        <v>12</v>
+      </c>
+      <c r="H64" t="s">
+        <v>12</v>
+      </c>
+      <c r="I64" t="s">
+        <v>12</v>
+      </c>
+      <c r="J64" t="s">
+        <v>12</v>
+      </c>
+      <c r="K64" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>